<commit_message>
Lots of changes, defining helper methods to use in a greater function call eventually
</commit_message>
<xml_diff>
--- a/nurse_schedule_project2_data_large_VA.xlsx
+++ b/nurse_schedule_project2_data_large_VA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RobertH/Desktop/ISE 3434/ISE 3434 - Project 1 - Submissions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcfro\Documents\GitHub\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120D60E2-3DB5-FF4C-80FE-485DB713F24A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F80274F-7ED0-4B6F-82C5-05F16B7B26EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="1" r:id="rId1"/>
@@ -1151,58 +1151,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1218,9 +1218,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>80</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>92</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>94</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>96</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>98</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>103</v>
       </c>
@@ -1637,13 +1637,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>106</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>111</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>119</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>120</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>122</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>124</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>125</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>127</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>131</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>132</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>135</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>137</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>139</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>140</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>142</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>144</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>146</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>148</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>150</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>151</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>152</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>153</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>154</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>155</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>157</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>159</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>160</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>162</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>163</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>164</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>165</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>167</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>168</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>169</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>170</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>171</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>173</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>174</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>176</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>178</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>180</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>181</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>183</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>184</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>185</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>186</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>187</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>189</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>190</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>192</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>194</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>195</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>196</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>197</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>198</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>199</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>200</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>202</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>204</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>205</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>206</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>207</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>208</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>210</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>211</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>213</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>214</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>215</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>217</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>219</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>221</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>222</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>224</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>225</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>226</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>228</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>229</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>230</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>231</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>232</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>233</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>234</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>236</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>237</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>238</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>239</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>240</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>241</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>242</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>244</v>
       </c>
@@ -3145,12 +3145,12 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>245</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>107</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -3217,9 +3217,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>